<commit_message>
build: Adding package psycopg2 and configure DB with docker compose.
</commit_message>
<xml_diff>
--- a/dados/planilhaAlunos.xlsx
+++ b/dados/planilhaAlunos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,71 +468,71 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Aprovado</t>
+          <t>Em Recuperação</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tati</t>
+          <t>Natan</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Aprovado</t>
+          <t>Em Recuperação</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Natan</t>
+          <t>Teste</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Natan</t>
+          <t>Tati</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -576,22 +576,184 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>Aprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Natan</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Em Recuperação</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Natan</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Em Recuperação</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Aprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>

</xml_diff>